<commit_message>
#Feature   - auto mail sender is updated
</commit_message>
<xml_diff>
--- a/emails/emails.xlsx
+++ b/emails/emails.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="570" windowWidth="28455" windowHeight="11955"/>
+  </bookViews>
   <sheets>
     <sheet name="email" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -375,92 +381,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>email</v>
-      </c>
-      <c r="B1" t="str">
-        <v>client_id</v>
-      </c>
-      <c r="C1" t="str">
-        <v>client_secret</v>
-      </c>
-      <c r="D1" t="str">
-        <v>redirect_uris</v>
-      </c>
-      <c r="E1" t="str">
-        <v>access_token</v>
-      </c>
-      <c r="F1" t="str">
-        <v>scope</v>
-      </c>
-      <c r="G1" t="str">
-        <v>token_type</v>
-      </c>
-      <c r="H1" t="str">
-        <v>expiry_date</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>woshikuzzaman@gmail.com</v>
-      </c>
-      <c r="B2" t="str">
-        <v>373325529411-n5oo39suh15qcps3a8276v5u51eiejdb.apps.googleusercontent.com</v>
-      </c>
-      <c r="C2" t="str">
-        <v>rZkZLLjNThBmxS_R-4gSFZbq</v>
-      </c>
-      <c r="D2" t="str">
-        <v>urn:ietf:wg:oauth:2.0:oob</v>
-      </c>
-      <c r="E2" t="str">
-        <v>ya29.Glt_B4FgTUIMwZVfM8dUOY-HrlqRxz1gd0rkJ6LRgookhBwTwjF840MIk3-z_thiRPMVts5QGLeo5EsNsS4g3BCgrvBDZsd4QxrfHkfMKemcZdDUPWjP7FExJSEl</v>
-      </c>
-      <c r="F2" t="str">
-        <v>https://mail.google.com/</v>
-      </c>
-      <c r="G2" t="str">
-        <v>Bearer</v>
-      </c>
-      <c r="H2">
-        <v>1568119382537</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>woshikuzzaman.cto@gmail.com</v>
-      </c>
-      <c r="B3" t="str">
-        <v>703598238217-r6h9ncdqfk52ai610avro7lrk3ecoen1.apps.googleusercontent.com</v>
-      </c>
-      <c r="C3" t="str">
-        <v>2EfI-BlsPaQm7JPBCluSv5Vv</v>
-      </c>
-      <c r="D3" t="str">
-        <v>urn:ietf:wg:oauth:2.0:oob</v>
-      </c>
-      <c r="E3" t="str">
-        <v>ya29.Glt_B1SUMry7h1PuG3b-MjYjwe7mlKTT-EE0SXwesnF4YU-S1BX82JO9t9H5DSxLXWzs2MgWeJfWqcRPCIGR_kYhy8DQsur_1R0KmbmvVVDeeNe7oQFxdDxPKxhE</v>
-      </c>
-      <c r="F3" t="str">
-        <v>https://mail.google.com/</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Bearer</v>
-      </c>
-      <c r="H3">
-        <v>1568119531300</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
-  </ignoredErrors>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#Feature   - new update
</commit_message>
<xml_diff>
--- a/emails/emails.xlsx
+++ b/emails/emails.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="570" windowWidth="28455" windowHeight="11955"/>
-  </bookViews>
   <sheets>
     <sheet name="email" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -381,14 +379,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>email</v>
+      </c>
+      <c r="B1" t="str">
+        <v>client_id</v>
+      </c>
+      <c r="C1" t="str">
+        <v>client_secret</v>
+      </c>
+      <c r="D1" t="str">
+        <v>redirect_uris</v>
+      </c>
+      <c r="E1" t="str">
+        <v>access_token</v>
+      </c>
+      <c r="F1" t="str">
+        <v>refresh_token</v>
+      </c>
+      <c r="G1" t="str">
+        <v>scope</v>
+      </c>
+      <c r="H1" t="str">
+        <v>token_type</v>
+      </c>
+      <c r="I1" t="str">
+        <v>expiry_date</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>alyssamarie69554@gmail.com</v>
+      </c>
+      <c r="B2" t="str">
+        <v>440677329044-5tb7ovk4h5gs19ktcfau55hqf192o86q.apps.googleusercontent.com</v>
+      </c>
+      <c r="C2" t="str">
+        <v>I6UAzzKNvJpBIG4MXAwpGh9U</v>
+      </c>
+      <c r="D2" t="str">
+        <v>urn:ietf:wg:oauth:2.0:oob</v>
+      </c>
+      <c r="E2" t="str">
+        <v>ya29.Il-EB1bTQsiCmYY8ve-xKDvVtXAmXLvZ9kt9InDE1wnk_7TUrqOAznuISim3c2iCfP7g9WXBFOrhdMXVS7JV3O89OShIJhvA82eYZ7vdut0ge3ZI1EUwPZl--D37px1-sg</v>
+      </c>
+      <c r="F2" t="str">
+        <v>1/PCbHoOKHgrk7f7moy_GFTUeKg8ZHYw6deBERYKMkhyg</v>
+      </c>
+      <c r="G2" t="str">
+        <v>https://mail.google.com/</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Bearer</v>
+      </c>
+      <c r="I2">
+        <v>1568523661006</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#Fix   - gmail smtp
</commit_message>
<xml_diff>
--- a/emails/emails.xlsx
+++ b/emails/emails.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,9 +442,38 @@
         <v>1568523661006</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>woshikuzzaman.cto@gmail.com</v>
+      </c>
+      <c r="B3" t="str">
+        <v>703598238217-r6h9ncdqfk52ai610avro7lrk3ecoen1.apps.googleusercontent.com</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2EfI-BlsPaQm7JPBCluSv5Vv</v>
+      </c>
+      <c r="D3" t="str">
+        <v>urn:ietf:wg:oauth:2.0:oob</v>
+      </c>
+      <c r="E3" t="str">
+        <v>ya29.Il-QB9llVMBnQgSejtY3zrxt5xO0nluRBzzTaJ-REh5yXuXsd0wPMKyG3IM2FJu-19qPykprVCCSAXDc69vLn3D4hD1IN3O905mXtt-vWCPNUdAmN68uKeOKS3PC_ro5vQ</v>
+      </c>
+      <c r="F3" t="str">
+        <v>1/C1w6bOVy0hzfa3i9R8LYt6HOMAWzr-hH9E6v7RJxdw0</v>
+      </c>
+      <c r="G3" t="str">
+        <v>https://mail.google.com/</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Bearer</v>
+      </c>
+      <c r="I3">
+        <v>1569611536145</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>